<commit_message>
Added document importing with automation for Organization appending as well as the emails have auto generated bodys with proper user tags and organization
</commit_message>
<xml_diff>
--- a/tabChecker/upload/attendeesupload.xlsx
+++ b/tabChecker/upload/attendeesupload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlesmeyer/Documents/TabCheck/tabChecker/upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42347876-ED3D-8F41-9083-225ED90BAEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AF8B61-2A9A-D447-8E6F-548339D7A60B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,19 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phonenumber</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Dylan</t>
   </si>
@@ -68,6 +56,33 @@
   </si>
   <si>
     <t>willwaters2019@gmail.com</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>+17068185081</t>
+  </si>
+  <si>
+    <t>+14789733746</t>
+  </si>
+  <si>
+    <t>+17063729685</t>
+  </si>
+  <si>
+    <t>+19123348897</t>
   </si>
 </sst>
 </file>
@@ -331,82 +346,97 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2">
-        <v>7068185081</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2">
-        <v>4789733746</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2">
-        <v>7063729685</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2">
-        <v>9123348897</v>
+      <c r="E5" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>